<commit_message>
agregando mas valores desde el excel
</commit_message>
<xml_diff>
--- a/PERSONAS.xlsx
+++ b/PERSONAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.rodriguez\Desktop\GenerarCertificadosEnPDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F837DF-4F03-4F4F-9FC3-A23D696863CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E220C6-5542-47CE-92A9-49202016A145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{31277DD1-BC3F-4127-9BE8-1D04CE796C4D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>nombreEstudiante</t>
   </si>
@@ -53,6 +53,24 @@
   </si>
   <si>
     <t>Luis Rodriguez</t>
+  </si>
+  <si>
+    <t>descripcionCurso</t>
+  </si>
+  <si>
+    <t>Prueba descripcion curso a ser buena persona</t>
+  </si>
+  <si>
+    <t>Cantidad horaria de 20 horas</t>
+  </si>
+  <si>
+    <t>duracionCurso</t>
+  </si>
+  <si>
+    <t>nombreCapacitador</t>
+  </si>
+  <si>
+    <t>Ing. Viviana Isabel Montes Sierra</t>
   </si>
 </sst>
 </file>
@@ -405,57 +423,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3A22D9-AB95-4A43-858B-DFD67F43741D}">
-  <dimension ref="B4:C8"/>
+  <dimension ref="B4:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
         <v>103659951</v>
       </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>326164978</v>
       </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
         <v>10937080</v>
       </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
         <v>60545</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>